<commit_message>
update EQU en cours
</commit_message>
<xml_diff>
--- a/TNR_PREJDD/PREJDD.RT.EQU.xlsx
+++ b/TNR_PREJDD/PREJDD.RT.EQU.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="223">
   <si>
     <t>Date</t>
   </si>
@@ -296,9 +296,6 @@
     <t>EQU02</t>
   </si>
   <si>
-    <t>EQU.RT.EQU.001.LEC.01</t>
-  </si>
-  <si>
     <t>MEREETFILLE</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     <t>EQU03</t>
   </si>
   <si>
-    <t>EQU.RT.EQU.001.MAJ.01</t>
-  </si>
-  <si>
     <t>PEREETFILS</t>
   </si>
   <si>
@@ -413,9 +407,6 @@
     <t>EQU04</t>
   </si>
   <si>
-    <t>EQU.RT.EQU.001.SUP.01</t>
-  </si>
-  <si>
     <t>REFFOU04</t>
   </si>
   <si>
@@ -450,9 +441,6 @@
   </si>
   <si>
     <t>EQU05</t>
-  </si>
-  <si>
-    <t>EQU.RT.EQU.001.REC.01</t>
   </si>
   <si>
     <t>REFFOU05</t>
@@ -2578,13 +2566,13 @@
       </c>
       <c r="Y2" s="17" t="str">
         <f t="shared" ref="Y2:Y16" si="1">CONCATENATE(UPPER(AA2),REPT(".",30-LEN(AA2)))</f>
-        <v>EQU.RT.EQU.001.LEC.01.........</v>
+        <v>RT.EQU.001.LEC.01.............</v>
       </c>
       <c r="Z2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="AA2" s="17" t="s">
-        <v>91</v>
+      <c r="AA2" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="AB2" s="20">
         <v>1001.0</v>
@@ -2595,23 +2583,23 @@
       <c r="AD2" s="20">
         <v>120.0</v>
       </c>
-      <c r="AE2" s="17" t="s">
-        <v>84</v>
+      <c r="AE2" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF2" s="21" t="s">
         <v>84</v>
       </c>
       <c r="AG2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AH2" s="17" t="s">
+      <c r="AI2" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="AJ2" s="17" t="s">
         <v>94</v>
-      </c>
-      <c r="AJ2" s="17" t="s">
-        <v>95</v>
       </c>
       <c r="AK2" s="22">
         <v>43922.0</v>
@@ -2623,7 +2611,7 @@
         <v>84</v>
       </c>
       <c r="AN2" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AO2" s="22">
         <v>44652.0</v>
@@ -2632,35 +2620,35 @@
         <v>20000.0</v>
       </c>
       <c r="AQ2" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AR2" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AS2" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AT2" s="18" t="str">
         <f t="shared" ref="AT2:AT16" si="2">Y2</f>
-        <v>EQU.RT.EQU.001.LEC.01.........</v>
+        <v>RT.EQU.001.LEC.01.............</v>
       </c>
       <c r="AU2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ2" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV2" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW2" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX2" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY2" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ2" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA2" s="20">
         <v>110000.0</v>
@@ -2672,10 +2660,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="BE2" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="BE2" s="23" t="s">
-        <v>100</v>
       </c>
       <c r="BF2" s="17" t="s">
         <v>84</v>
@@ -2684,7 +2672,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH2" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI2" s="17" t="s">
         <v>84</v>
@@ -2693,36 +2681,36 @@
         <v>1000.0</v>
       </c>
       <c r="BK2" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="BL2" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="BM2" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="BN2" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="BL2" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="BM2" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="BN2" s="25" t="s">
-        <v>103</v>
-      </c>
       <c r="BO2" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="15">
         <v>1001.0</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>106</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>107</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>84</v>
@@ -2752,7 +2740,7 @@
         <v>84</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>85</v>
@@ -2764,16 +2752,16 @@
         <v>84</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T3" s="19">
         <v>0.0</v>
       </c>
       <c r="U3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="V3" s="16" t="s">
         <v>110</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>111</v>
       </c>
       <c r="W3" s="19">
         <v>1.0</v>
@@ -2783,13 +2771,13 @@
       </c>
       <c r="Y3" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>EQU.RT.EQU.001.MAJ.01.........</v>
+        <v>RT.EQU.001.MAJ.01.............</v>
       </c>
       <c r="Z3" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="AA3" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="AB3" s="20">
         <v>1003.0</v>
@@ -2800,23 +2788,23 @@
       <c r="AD3" s="27">
         <v>130.0</v>
       </c>
-      <c r="AE3" s="17" t="s">
-        <v>84</v>
+      <c r="AE3" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF3" s="21" t="s">
         <v>84</v>
       </c>
       <c r="AG3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH3" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI3" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="AH3" s="16" t="s">
+      <c r="AJ3" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="AI3" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ3" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="AK3" s="28">
         <v>43466.0</v>
@@ -2828,7 +2816,7 @@
         <v>84</v>
       </c>
       <c r="AN3" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AO3" s="22">
         <v>43831.0</v>
@@ -2837,23 +2825,23 @@
         <v>30000.0</v>
       </c>
       <c r="AQ3" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR3" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS3" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT3" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>EQU.RT.EQU.001.MAJ.01.........</v>
+        <v>RT.EQU.001.MAJ.01.............</v>
       </c>
       <c r="AU3" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AV3" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AW3" s="17" t="s">
         <v>84</v>
@@ -2865,7 +2853,7 @@
         <v>84</v>
       </c>
       <c r="AZ3" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA3" s="27">
         <v>200000.0</v>
@@ -2877,10 +2865,10 @@
         <v>4000000.0</v>
       </c>
       <c r="BD3" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BE3" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BF3" s="17" t="s">
         <v>84</v>
@@ -2889,7 +2877,7 @@
         <v>43831.0</v>
       </c>
       <c r="BH3" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI3" s="17" t="s">
         <v>84</v>
@@ -2898,36 +2886,36 @@
         <v>1002.0</v>
       </c>
       <c r="BK3" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="BL3" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM3" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN3" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO3" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="15">
         <v>1002.0</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>124</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>84</v>
@@ -2957,7 +2945,7 @@
         <v>84</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P4" s="16" t="s">
         <v>85</v>
@@ -2969,16 +2957,16 @@
         <v>84</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="T4" s="19">
         <v>0.0</v>
       </c>
       <c r="U4" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="V4" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="W4" s="19">
         <v>1.0</v>
@@ -2988,13 +2976,13 @@
       </c>
       <c r="Y4" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>EQU.RT.EQU.001.SUP.01.........</v>
+        <v>RT.EQU.001.SUP.01.............</v>
       </c>
       <c r="Z4" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AA4" s="16" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="AB4" s="27">
         <v>1004.0</v>
@@ -3005,23 +2993,23 @@
       <c r="AD4" s="21">
         <v>140.0</v>
       </c>
-      <c r="AE4" s="17" t="s">
-        <v>84</v>
+      <c r="AE4" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF4" s="21" t="s">
         <v>84</v>
       </c>
       <c r="AG4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AH4" s="17" t="s">
+      <c r="AI4" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="AI4" s="17" t="s">
-        <v>94</v>
-      </c>
       <c r="AJ4" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AK4" s="28">
         <v>43466.0</v>
@@ -3033,7 +3021,7 @@
         <v>84</v>
       </c>
       <c r="AN4" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AO4" s="22">
         <v>43831.0</v>
@@ -3042,35 +3030,35 @@
         <v>40000.0</v>
       </c>
       <c r="AQ4" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AR4" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AS4" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AT4" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>EQU.RT.EQU.001.SUP.01.........</v>
+        <v>RT.EQU.001.SUP.01.............</v>
       </c>
       <c r="AU4" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV4" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW4" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX4" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY4" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ4" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV4" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW4" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX4" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY4" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ4" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA4" s="20">
         <v>290000.0</v>
@@ -3082,10 +3070,10 @@
         <v>6000000.0</v>
       </c>
       <c r="BD4" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BE4" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="BF4" s="17" t="s">
         <v>84</v>
@@ -3094,7 +3082,7 @@
         <v>43831.0</v>
       </c>
       <c r="BH4" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI4" s="17" t="s">
         <v>84</v>
@@ -3103,36 +3091,36 @@
         <v>1004.0</v>
       </c>
       <c r="BK4" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BL4" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM4" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B5" s="15">
         <v>1003.0</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>84</v>
@@ -3162,7 +3150,7 @@
         <v>84</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="P5" s="16" t="s">
         <v>85</v>
@@ -3174,7 +3162,7 @@
         <v>84</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="T5" s="19">
         <v>0.0</v>
@@ -3183,7 +3171,7 @@
         <v>88</v>
       </c>
       <c r="V5" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="W5" s="19">
         <v>1.0</v>
@@ -3193,13 +3181,13 @@
       </c>
       <c r="Y5" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>EQU.RT.EQU.001.REC.01.........</v>
+        <v>RT.EQU.001.REC.01.............</v>
       </c>
       <c r="Z5" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AA5" s="16" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="AB5" s="27">
         <v>1005.0</v>
@@ -3210,23 +3198,23 @@
       <c r="AD5" s="21">
         <v>150.0</v>
       </c>
-      <c r="AE5" s="17" t="s">
-        <v>84</v>
+      <c r="AE5" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF5" s="21" t="s">
         <v>84</v>
       </c>
       <c r="AG5" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH5" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI5" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="AH5" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI5" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="AJ5" s="16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="AK5" s="28">
         <v>43466.0</v>
@@ -3238,7 +3226,7 @@
         <v>84</v>
       </c>
       <c r="AN5" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AO5" s="22">
         <v>43831.0</v>
@@ -3247,23 +3235,23 @@
         <v>50000.0</v>
       </c>
       <c r="AQ5" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR5" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS5" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT5" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>EQU.RT.EQU.001.REC.01.........</v>
+        <v>RT.EQU.001.REC.01.............</v>
       </c>
       <c r="AU5" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AV5" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AW5" s="17" t="s">
         <v>84</v>
@@ -3275,7 +3263,7 @@
         <v>84</v>
       </c>
       <c r="AZ5" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA5" s="27">
         <v>380000.0</v>
@@ -3287,10 +3275,10 @@
         <v>8000000.0</v>
       </c>
       <c r="BD5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="BE5" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="BE5" s="23" t="s">
-        <v>100</v>
       </c>
       <c r="BF5" s="17" t="s">
         <v>84</v>
@@ -3299,7 +3287,7 @@
         <v>43831.0</v>
       </c>
       <c r="BH5" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI5" s="17" t="s">
         <v>84</v>
@@ -3308,24 +3296,24 @@
         <v>1005.0</v>
       </c>
       <c r="BK5" s="16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="BL5" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM5" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN5" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO5" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B6" s="15">
         <v>1004.0</v>
@@ -3388,7 +3376,7 @@
         <v>88</v>
       </c>
       <c r="V6" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="W6" s="19">
         <v>1.0</v>
@@ -3401,10 +3389,10 @@
         <v>EQU.RT.ART.006.SRA.01.........</v>
       </c>
       <c r="Z6" s="17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="AA6" s="21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="AB6" s="21">
         <v>1006.0</v>
@@ -3415,8 +3403,8 @@
       <c r="AD6" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE6" s="17" t="s">
-        <v>84</v>
+      <c r="AE6" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF6" s="21" t="s">
         <v>84</v>
@@ -3443,7 +3431,7 @@
         <v>84</v>
       </c>
       <c r="AN6" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AO6" s="22">
         <v>43831.0</v>
@@ -3452,35 +3440,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ6" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR6" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS6" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT6" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.RT.ART.006.SRA.01.........</v>
       </c>
       <c r="AU6" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV6" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ6" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV6" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW6" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX6" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY6" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ6" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA6" s="27">
         <v>380000.0</v>
@@ -3492,10 +3480,10 @@
         <v>8000000.0</v>
       </c>
       <c r="BD6" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BE6" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BF6" s="17" t="s">
         <v>84</v>
@@ -3504,7 +3492,7 @@
         <v>43831.0</v>
       </c>
       <c r="BH6" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI6" s="17" t="s">
         <v>84</v>
@@ -3516,21 +3504,21 @@
         <v>84</v>
       </c>
       <c r="BL6" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM6" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN6" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO6" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B7" s="15">
         <v>1005.0</v>
@@ -3593,7 +3581,7 @@
         <v>88</v>
       </c>
       <c r="V7" s="16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="W7" s="19">
         <v>1.0</v>
@@ -3606,10 +3594,10 @@
         <v>EQU.RT.MAT.001.CRE.01.........</v>
       </c>
       <c r="Z7" s="17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="AA7" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AB7" s="21">
         <v>1007.0</v>
@@ -3620,8 +3608,8 @@
       <c r="AD7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE7" s="17" t="s">
-        <v>84</v>
+      <c r="AE7" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF7" s="21" t="s">
         <v>84</v>
@@ -3648,7 +3636,7 @@
         <v>84</v>
       </c>
       <c r="AN7" s="16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AO7" s="22">
         <v>43831.0</v>
@@ -3657,35 +3645,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ7" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR7" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS7" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT7" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.RT.MAT.001.CRE.01.........</v>
       </c>
       <c r="AU7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ7" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV7" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW7" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX7" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY7" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ7" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA7" s="27">
         <v>380000.0</v>
@@ -3697,10 +3685,10 @@
         <v>8000000.0</v>
       </c>
       <c r="BD7" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BE7" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="BF7" s="17" t="s">
         <v>84</v>
@@ -3709,7 +3697,7 @@
         <v>43831.0</v>
       </c>
       <c r="BH7" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI7" s="17" t="s">
         <v>84</v>
@@ -3721,21 +3709,21 @@
         <v>84</v>
       </c>
       <c r="BL7" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM7" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN7" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO7" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B8" s="15">
         <v>1006.0</v>
@@ -3795,10 +3783,10 @@
         <v>0.0</v>
       </c>
       <c r="U8" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V8" s="17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="W8" s="19">
         <v>1.0</v>
@@ -3811,10 +3799,10 @@
         <v>EQU.TR.BTR.001.CRE.01.........</v>
       </c>
       <c r="Z8" s="17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="AA8" s="17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AB8" s="21">
         <v>1008.0</v>
@@ -3825,8 +3813,8 @@
       <c r="AD8" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE8" s="17" t="s">
-        <v>84</v>
+      <c r="AE8" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF8" s="21" t="s">
         <v>84</v>
@@ -3853,7 +3841,7 @@
         <v>84</v>
       </c>
       <c r="AN8" s="16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AO8" s="22">
         <v>43831.0</v>
@@ -3862,35 +3850,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ8" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR8" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS8" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT8" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.TR.BTR.001.CRE.01.........</v>
       </c>
       <c r="AU8" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV8" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ8" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV8" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ8" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA8" s="20">
         <v>110000.0</v>
@@ -3902,10 +3890,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD8" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="BE8" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="BE8" s="23" t="s">
-        <v>100</v>
       </c>
       <c r="BF8" s="17" t="s">
         <v>84</v>
@@ -3914,7 +3902,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH8" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI8" s="17" t="s">
         <v>84</v>
@@ -3926,21 +3914,21 @@
         <v>84</v>
       </c>
       <c r="BL8" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM8" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN8" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO8" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="33" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B9" s="15">
         <v>1007.0</v>
@@ -4000,10 +3988,10 @@
         <v>0.0</v>
       </c>
       <c r="U9" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V9" s="16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="W9" s="19">
         <v>1.0</v>
@@ -4016,10 +4004,10 @@
         <v>EQU.TR.BTR.001.CRE.03.........</v>
       </c>
       <c r="Z9" s="17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="AA9" s="17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="AB9" s="21">
         <v>1009.0</v>
@@ -4030,8 +4018,8 @@
       <c r="AD9" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE9" s="17" t="s">
-        <v>84</v>
+      <c r="AE9" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF9" s="21" t="s">
         <v>84</v>
@@ -4058,7 +4046,7 @@
         <v>84</v>
       </c>
       <c r="AN9" s="16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AO9" s="22">
         <v>43831.0</v>
@@ -4067,35 +4055,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ9" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR9" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS9" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT9" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.TR.BTR.001.CRE.03.........</v>
       </c>
       <c r="AU9" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV9" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ9" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV9" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW9" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX9" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY9" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ9" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA9" s="20">
         <v>110000.0</v>
@@ -4107,10 +4095,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD9" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BE9" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BF9" s="17" t="s">
         <v>84</v>
@@ -4119,7 +4107,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH9" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI9" s="17" t="s">
         <v>84</v>
@@ -4131,21 +4119,21 @@
         <v>84</v>
       </c>
       <c r="BL9" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM9" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN9" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO9" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="33" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B10" s="15">
         <v>1008.0</v>
@@ -4205,10 +4193,10 @@
         <v>0.0</v>
       </c>
       <c r="U10" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V10" s="17" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="W10" s="19">
         <v>1.0</v>
@@ -4221,10 +4209,10 @@
         <v>EQU.TR.BTR.001.LEC.01.........</v>
       </c>
       <c r="Z10" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="AA10" s="17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AB10" s="21">
         <v>1010.0</v>
@@ -4235,8 +4223,8 @@
       <c r="AD10" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE10" s="17" t="s">
-        <v>84</v>
+      <c r="AE10" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF10" s="21" t="s">
         <v>84</v>
@@ -4263,7 +4251,7 @@
         <v>84</v>
       </c>
       <c r="AN10" s="16" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AO10" s="22">
         <v>43831.0</v>
@@ -4272,35 +4260,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ10" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR10" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS10" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT10" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.TR.BTR.001.LEC.01.........</v>
       </c>
       <c r="AU10" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV10" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ10" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV10" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW10" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX10" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY10" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ10" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA10" s="20">
         <v>110000.0</v>
@@ -4312,10 +4300,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD10" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BE10" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="BF10" s="17" t="s">
         <v>84</v>
@@ -4324,7 +4312,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH10" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI10" s="17" t="s">
         <v>84</v>
@@ -4336,21 +4324,21 @@
         <v>84</v>
       </c>
       <c r="BL10" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM10" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN10" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO10" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="33" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B11" s="15">
         <v>1009.0</v>
@@ -4410,10 +4398,10 @@
         <v>0.0</v>
       </c>
       <c r="U11" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V11" s="16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="W11" s="19">
         <v>1.0</v>
@@ -4426,10 +4414,10 @@
         <v>EQU.UPD.TR.BTR.001.MAJ.01.....</v>
       </c>
       <c r="Z11" s="17" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="AA11" s="17" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AB11" s="21">
         <v>1011.0</v>
@@ -4440,8 +4428,8 @@
       <c r="AD11" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE11" s="17" t="s">
-        <v>84</v>
+      <c r="AE11" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF11" s="21" t="s">
         <v>84</v>
@@ -4468,7 +4456,7 @@
         <v>84</v>
       </c>
       <c r="AN11" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AO11" s="22">
         <v>43831.0</v>
@@ -4477,35 +4465,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ11" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR11" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS11" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT11" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.UPD.TR.BTR.001.MAJ.01.....</v>
       </c>
       <c r="AU11" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV11" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW11" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX11" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY11" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ11" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV11" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW11" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX11" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY11" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ11" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA11" s="20">
         <v>110000.0</v>
@@ -4517,10 +4505,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD11" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="BE11" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="BE11" s="23" t="s">
-        <v>100</v>
       </c>
       <c r="BF11" s="17" t="s">
         <v>84</v>
@@ -4529,7 +4517,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH11" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI11" s="17" t="s">
         <v>84</v>
@@ -4541,21 +4529,21 @@
         <v>84</v>
       </c>
       <c r="BL11" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM11" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN11" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO11" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="33" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B12" s="15">
         <v>1010.0</v>
@@ -4615,10 +4603,10 @@
         <v>0.0</v>
       </c>
       <c r="U12" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V12" s="16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="W12" s="19">
         <v>1.0</v>
@@ -4631,10 +4619,10 @@
         <v>EQU.TR.BTR.001.MAJ.01.........</v>
       </c>
       <c r="Z12" s="17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="AA12" s="17" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AB12" s="21">
         <v>1012.0</v>
@@ -4645,8 +4633,8 @@
       <c r="AD12" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE12" s="17" t="s">
-        <v>84</v>
+      <c r="AE12" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF12" s="21" t="s">
         <v>84</v>
@@ -4673,7 +4661,7 @@
         <v>84</v>
       </c>
       <c r="AN12" s="16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="AO12" s="22">
         <v>43831.0</v>
@@ -4682,35 +4670,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ12" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR12" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS12" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT12" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.TR.BTR.001.MAJ.01.........</v>
       </c>
       <c r="AU12" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV12" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW12" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX12" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY12" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ12" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV12" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW12" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX12" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY12" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ12" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA12" s="20">
         <v>110000.0</v>
@@ -4722,10 +4710,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD12" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BE12" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BF12" s="17" t="s">
         <v>84</v>
@@ -4734,7 +4722,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH12" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI12" s="17" t="s">
         <v>84</v>
@@ -4746,21 +4734,21 @@
         <v>84</v>
       </c>
       <c r="BL12" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM12" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN12" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO12" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B13" s="15">
         <v>1011.0</v>
@@ -4820,10 +4808,10 @@
         <v>0.0</v>
       </c>
       <c r="U13" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V13" s="16" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="W13" s="19">
         <v>1.0</v>
@@ -4836,10 +4824,10 @@
         <v>EQU.TR.BTR.001.SUP.01.........</v>
       </c>
       <c r="Z13" s="17" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="AA13" s="17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="AB13" s="21">
         <v>1013.0</v>
@@ -4850,8 +4838,8 @@
       <c r="AD13" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE13" s="17" t="s">
-        <v>84</v>
+      <c r="AE13" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF13" s="21" t="s">
         <v>84</v>
@@ -4878,7 +4866,7 @@
         <v>84</v>
       </c>
       <c r="AN13" s="16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="AO13" s="22">
         <v>43831.0</v>
@@ -4887,35 +4875,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT13" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.TR.BTR.001.SUP.01.........</v>
       </c>
       <c r="AU13" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV13" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW13" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX13" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY13" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ13" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV13" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW13" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX13" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY13" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ13" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA13" s="20">
         <v>110000.0</v>
@@ -4927,10 +4915,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD13" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BE13" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="BF13" s="17" t="s">
         <v>84</v>
@@ -4939,7 +4927,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH13" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI13" s="17" t="s">
         <v>84</v>
@@ -4951,21 +4939,21 @@
         <v>84</v>
       </c>
       <c r="BL13" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM13" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN13" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO13" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B14" s="15">
         <v>1012.0</v>
@@ -5025,10 +5013,10 @@
         <v>0.0</v>
       </c>
       <c r="U14" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V14" s="17" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="W14" s="19">
         <v>1.0</v>
@@ -5041,10 +5029,10 @@
         <v>EQU.TR.BTR.001.REC.01.........</v>
       </c>
       <c r="Z14" s="17" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="AA14" s="17" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="AB14" s="21">
         <v>1014.0</v>
@@ -5055,8 +5043,8 @@
       <c r="AD14" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE14" s="17" t="s">
-        <v>84</v>
+      <c r="AE14" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF14" s="21" t="s">
         <v>84</v>
@@ -5083,7 +5071,7 @@
         <v>84</v>
       </c>
       <c r="AN14" s="16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="AO14" s="22">
         <v>43831.0</v>
@@ -5092,35 +5080,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ14" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR14" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS14" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT14" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.TR.BTR.001.REC.01.........</v>
       </c>
       <c r="AU14" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV14" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW14" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX14" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY14" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ14" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV14" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW14" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX14" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY14" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ14" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA14" s="20">
         <v>110000.0</v>
@@ -5132,10 +5120,10 @@
         <v>2000000.0</v>
       </c>
       <c r="BD14" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="BE14" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="BE14" s="23" t="s">
-        <v>100</v>
       </c>
       <c r="BF14" s="17" t="s">
         <v>84</v>
@@ -5144,7 +5132,7 @@
         <v>44652.0</v>
       </c>
       <c r="BH14" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI14" s="17" t="s">
         <v>84</v>
@@ -5156,21 +5144,21 @@
         <v>84</v>
       </c>
       <c r="BL14" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM14" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN14" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO14" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="33" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B15" s="15">
         <v>1013.0</v>
@@ -5233,7 +5221,7 @@
         <v>88</v>
       </c>
       <c r="V15" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="W15" s="19">
         <v>1.0</v>
@@ -5246,10 +5234,10 @@
         <v>EQU.RT.ART.006.SRM.01.........</v>
       </c>
       <c r="Z15" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AA15" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AB15" s="21">
         <v>1015.0</v>
@@ -5260,8 +5248,8 @@
       <c r="AD15" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE15" s="17" t="s">
-        <v>84</v>
+      <c r="AE15" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF15" s="21" t="s">
         <v>84</v>
@@ -5288,7 +5276,7 @@
         <v>84</v>
       </c>
       <c r="AN15" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AO15" s="22">
         <v>43831.0</v>
@@ -5297,35 +5285,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ15" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR15" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS15" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT15" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.RT.ART.006.SRM.01.........</v>
       </c>
       <c r="AU15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW15" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX15" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY15" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ15" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV15" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW15" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX15" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY15" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ15" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA15" s="27">
         <v>380000.0</v>
@@ -5337,10 +5325,10 @@
         <v>8000000.0</v>
       </c>
       <c r="BD15" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BE15" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BF15" s="17" t="s">
         <v>84</v>
@@ -5349,7 +5337,7 @@
         <v>43831.0</v>
       </c>
       <c r="BH15" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI15" s="17" t="s">
         <v>84</v>
@@ -5361,21 +5349,21 @@
         <v>84</v>
       </c>
       <c r="BL15" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM15" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN15" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO15" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B16" s="15">
         <v>1014.0</v>
@@ -5438,7 +5426,7 @@
         <v>88</v>
       </c>
       <c r="V16" s="17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="W16" s="19">
         <v>1.0</v>
@@ -5451,10 +5439,10 @@
         <v>EQU.RT.ART.006.SRS.01.........</v>
       </c>
       <c r="Z16" s="17" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AA16" s="17" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="AB16" s="21">
         <v>1016.0</v>
@@ -5465,8 +5453,8 @@
       <c r="AD16" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AE16" s="17" t="s">
-        <v>84</v>
+      <c r="AE16" s="16">
+        <v>0.0</v>
       </c>
       <c r="AF16" s="21" t="s">
         <v>84</v>
@@ -5493,7 +5481,7 @@
         <v>84</v>
       </c>
       <c r="AN16" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AO16" s="22">
         <v>43831.0</v>
@@ -5502,35 +5490,35 @@
         <v>50000.0</v>
       </c>
       <c r="AQ16" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR16" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AS16" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AT16" s="18" t="str">
         <f t="shared" si="2"/>
         <v>EQU.RT.ART.006.SRS.01.........</v>
       </c>
       <c r="AU16" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV16" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW16" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX16" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY16" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ16" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="AV16" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW16" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX16" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY16" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ16" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="BA16" s="27">
         <v>380000.0</v>
@@ -5542,10 +5530,10 @@
         <v>8000000.0</v>
       </c>
       <c r="BD16" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BE16" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="BF16" s="17" t="s">
         <v>84</v>
@@ -5554,7 +5542,7 @@
         <v>43831.0</v>
       </c>
       <c r="BH16" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI16" s="17" t="s">
         <v>84</v>
@@ -5566,16 +5554,16 @@
         <v>84</v>
       </c>
       <c r="BL16" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BM16" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BN16" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BO16" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -6991,7 +6979,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>14</v>
@@ -7000,10 +6988,10 @@
         <v>28</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -10047,19 +10035,19 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F1" s="36" t="s">
         <v>52</v>
@@ -10087,42 +10075,42 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B2" s="19">
         <v>1013.0</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E2" s="21">
         <v>10.0</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B3" s="19">
         <v>1014.0</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E3" s="21">
         <v>10.0</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -13138,13 +13126,13 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -13178,40 +13166,40 @@
         <v>1000.0</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="19">
         <v>1001.0</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="30">
         <v>1002.0</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B5" s="30">
         <v>1003.0</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -13222,40 +13210,40 @@
         <v>2000.0</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="19">
         <v>2001.0</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" s="19">
         <v>2002.0</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B9" s="19">
         <v>2003.0</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -13266,40 +13254,40 @@
         <v>3000.0</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="19">
         <v>3001.0</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12" s="19">
         <v>3002.0</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B13" s="19">
         <v>3003.0</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -16296,10 +16284,10 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>

</xml_diff>